<commit_message>
Ajout ModeExercice du professionnel 507063d4a882e3fa82fc6d0f1b3573519d0670e8
</commit_message>
<xml_diff>
--- a/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-practitioner-role.xlsx
+++ b/298-Ajout-de-l'évènement/ig/StructureDefinition-tddui-practitioner-role.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1915" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="367">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-24T08:59:11+00:00</t>
+    <t>2025-09-24T09:13:07+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -650,6 +650,25 @@
 </t>
   </si>
   <si>
+    <t>PractitionerRole.extension:TDDUIProfession</t>
+  </si>
+  <si>
+    <t>TDDUIProfession</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-exercise-mode}
+</t>
+  </si>
+  <si>
+    <t>Mode d'exercice</t>
+  </si>
+  <si>
+    <t>Extension permettant de représenter le mode d'exercice du professionnel.</t>
+  </si>
+  <si>
+    <t>modeExercice</t>
+  </si>
+  <si>
     <t>PractitionerRole.modifierExtension</t>
   </si>
   <si>
@@ -825,10 +844,7 @@
     <t>PractitionerRole.code.extension</t>
   </si>
   <si>
-    <t>PractitionerRole.code.extension:tddui-profession</t>
-  </si>
-  <si>
-    <t>tddui-profession</t>
+    <t>PractitionerRole.code.extension:TDDUIProfession</t>
   </si>
   <si>
     <t xml:space="preserve">Extension {https://interop.esante.gouv.fr/ig/fhir/tddui/StructureDefinition/tddui-profession}
@@ -1445,7 +1461,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO51"/>
+  <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1464,7 +1480,7 @@
     <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="73.4375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="76.2265625" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -3724,43 +3740,41 @@
         <v>204</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>204</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>194</v>
+      </c>
+      <c r="C20" t="s" s="2">
+        <v>205</v>
+      </c>
       <c r="D20" t="s" s="2">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G20" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H20" t="s" s="2">
         <v>78</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="J20" t="s" s="2">
         <v>78</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>111</v>
+        <v>206</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>114</v>
-      </c>
-      <c r="O20" t="s" s="2">
-        <v>207</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
         <v>78</v>
       </c>
@@ -3808,7 +3822,7 @@
         <v>78</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>79</v>
@@ -3823,13 +3837,13 @@
         <v>119</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>78</v>
+        <v>209</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>193</v>
+        <v>78</v>
       </c>
       <c r="AN20" t="s" s="2">
         <v>78</v>
@@ -3840,14 +3854,14 @@
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" t="s" s="2">
@@ -3860,13 +3874,13 @@
         <v>78</v>
       </c>
       <c r="I21" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>210</v>
+        <v>111</v>
       </c>
       <c r="L21" t="s" s="2">
         <v>211</v>
@@ -3874,7 +3888,9 @@
       <c r="M21" t="s" s="2">
         <v>212</v>
       </c>
-      <c r="N21" s="2"/>
+      <c r="N21" t="s" s="2">
+        <v>114</v>
+      </c>
       <c r="O21" t="s" s="2">
         <v>213</v>
       </c>
@@ -3925,7 +3941,7 @@
         <v>78</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>79</v>
@@ -3937,30 +3953,30 @@
         <v>78</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>214</v>
+        <v>78</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>216</v>
+        <v>78</v>
       </c>
       <c r="AO21" t="s" s="2">
-        <v>217</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -3971,7 +3987,7 @@
         <v>79</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>78</v>
@@ -3983,26 +3999,22 @@
         <v>91</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="N22" s="2"/>
+      <c r="O22" t="s" s="2">
         <v>219</v>
       </c>
-      <c r="L22" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="O22" t="s" s="2">
-        <v>223</v>
-      </c>
       <c r="P22" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="Q22" t="s" s="2">
-        <v>224</v>
-      </c>
+      <c r="Q22" s="2"/>
       <c r="R22" t="s" s="2">
         <v>78</v>
       </c>
@@ -4046,13 +4058,13 @@
         <v>78</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH22" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI22" t="s" s="2">
         <v>78</v>
@@ -4064,24 +4076,24 @@
         <v>78</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>78</v>
+        <v>222</v>
       </c>
       <c r="AO22" t="s" s="2">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4104,22 +4116,26 @@
         <v>91</v>
       </c>
       <c r="K23" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="L23" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="N23" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="O23" t="s" s="2">
         <v>229</v>
       </c>
-      <c r="L23" t="s" s="2">
+      <c r="P23" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Q23" t="s" s="2">
         <v>230</v>
       </c>
-      <c r="M23" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="N23" s="2"/>
-      <c r="O23" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="P23" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Q23" s="2"/>
       <c r="R23" t="s" s="2">
         <v>78</v>
       </c>
@@ -4163,7 +4179,7 @@
         <v>78</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>79</v>
@@ -4181,24 +4197,24 @@
         <v>78</v>
       </c>
       <c r="AL23" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="AM23" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="AN23" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AO23" t="s" s="2">
         <v>233</v>
-      </c>
-      <c r="AM23" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="AN23" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="AO23" t="s" s="2">
-        <v>236</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4221,16 +4237,18 @@
         <v>91</v>
       </c>
       <c r="K24" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L24" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="M24" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="N24" s="2"/>
+      <c r="O24" t="s" s="2">
         <v>238</v>
       </c>
-      <c r="L24" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
         <v>78</v>
       </c>
@@ -4278,7 +4296,7 @@
         <v>78</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>79</v>
@@ -4296,24 +4314,24 @@
         <v>78</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>78</v>
+        <v>239</v>
       </c>
       <c r="AM24" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="AN24" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="AN24" t="s" s="2">
-        <v>78</v>
-      </c>
       <c r="AO24" t="s" s="2">
-        <v>78</v>
+        <v>242</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -4336,13 +4354,13 @@
         <v>91</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -4393,7 +4411,7 @@
         <v>78</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>79</v>
@@ -4408,7 +4426,7 @@
         <v>102</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>246</v>
+        <v>78</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>78</v>
@@ -4459,12 +4477,8 @@
       <c r="M26" t="s" s="2">
         <v>251</v>
       </c>
-      <c r="N26" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="O26" t="s" s="2">
-        <v>253</v>
-      </c>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
         <v>78</v>
       </c>
@@ -4488,11 +4502,13 @@
         <v>78</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>174</v>
-      </c>
-      <c r="Y26" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="Y26" t="s" s="2">
+        <v>78</v>
+      </c>
       <c r="Z26" t="s" s="2">
-        <v>254</v>
+        <v>78</v>
       </c>
       <c r="AA26" t="s" s="2">
         <v>78</v>
@@ -4516,7 +4532,7 @@
         <v>79</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>78</v>
@@ -4525,16 +4541,16 @@
         <v>102</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>256</v>
+        <v>78</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>235</v>
+        <v>78</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>78</v>
@@ -4542,10 +4558,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -4565,19 +4581,23 @@
         <v>78</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>104</v>
+        <v>255</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>105</v>
+        <v>256</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
+        <v>257</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="O27" t="s" s="2">
+        <v>259</v>
+      </c>
       <c r="P27" t="s" s="2">
         <v>78</v>
       </c>
@@ -4601,13 +4621,11 @@
         <v>78</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Y27" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>174</v>
+      </c>
+      <c r="Y27" s="2"/>
       <c r="Z27" t="s" s="2">
-        <v>78</v>
+        <v>260</v>
       </c>
       <c r="AA27" t="s" s="2">
         <v>78</v>
@@ -4625,31 +4643,31 @@
         <v>78</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>107</v>
+        <v>254</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>78</v>
+        <v>261</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>78</v>
+        <v>262</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>108</v>
+        <v>263</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>78</v>
+        <v>241</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>78</v>
@@ -4657,21 +4675,21 @@
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>259</v>
+        <v>264</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G28" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H28" t="s" s="2">
         <v>78</v>
@@ -4683,17 +4701,15 @@
         <v>78</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="N28" t="s" s="2">
-        <v>114</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="N28" s="2"/>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
         <v>78</v>
@@ -4730,31 +4746,31 @@
         <v>78</v>
       </c>
       <c r="AB28" t="s" s="2">
-        <v>115</v>
+        <v>78</v>
       </c>
       <c r="AC28" t="s" s="2">
-        <v>116</v>
+        <v>78</v>
       </c>
       <c r="AD28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="AK28" t="s" s="2">
         <v>78</v>
@@ -4774,23 +4790,21 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="C29" t="s" s="2">
-        <v>261</v>
-      </c>
+        <v>265</v>
+      </c>
+      <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
-        <v>78</v>
+        <v>110</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G29" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H29" t="s" s="2">
         <v>78</v>
@@ -4802,15 +4816,17 @@
         <v>78</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>262</v>
+        <v>111</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>263</v>
+        <v>112</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>113</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>114</v>
+      </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s" s="2">
         <v>78</v>
@@ -4847,16 +4863,16 @@
         <v>78</v>
       </c>
       <c r="AB29" t="s" s="2">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="AC29" t="s" s="2">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="AD29" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>78</v>
+        <v>117</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>118</v>
@@ -4874,13 +4890,13 @@
         <v>119</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>265</v>
+        <v>78</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>78</v>
+        <v>108</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>78</v>
@@ -4894,9 +4910,11 @@
         <v>266</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="C30" s="2"/>
+        <v>265</v>
+      </c>
+      <c r="C30" t="s" s="2">
+        <v>205</v>
+      </c>
       <c r="D30" t="s" s="2">
         <v>78</v>
       </c>
@@ -4905,7 +4923,7 @@
         <v>79</v>
       </c>
       <c r="G30" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H30" t="s" s="2">
         <v>78</v>
@@ -4914,23 +4932,19 @@
         <v>78</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>148</v>
+        <v>267</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="N30" t="s" s="2">
         <v>269</v>
       </c>
-      <c r="O30" t="s" s="2">
-        <v>270</v>
-      </c>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
       <c r="P30" t="s" s="2">
         <v>78</v>
       </c>
@@ -4954,11 +4968,13 @@
         <v>78</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="Y30" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="Y30" t="s" s="2">
+        <v>78</v>
+      </c>
       <c r="Z30" t="s" s="2">
-        <v>272</v>
+        <v>78</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>78</v>
@@ -4976,7 +4992,7 @@
         <v>78</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>273</v>
+        <v>118</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>79</v>
@@ -4988,16 +5004,16 @@
         <v>78</v>
       </c>
       <c r="AJ30" t="s" s="2">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>78</v>
+        <v>270</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>274</v>
+        <v>78</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>275</v>
+        <v>78</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>78</v>
@@ -5008,10 +5024,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5022,7 +5038,7 @@
         <v>79</v>
       </c>
       <c r="G31" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H31" t="s" s="2">
         <v>78</v>
@@ -5034,19 +5050,19 @@
         <v>91</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>104</v>
+        <v>148</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="N31" t="s" s="2">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="O31" t="s" s="2">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>78</v>
@@ -5071,13 +5087,11 @@
         <v>78</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Y31" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="Y31" s="2"/>
       <c r="Z31" t="s" s="2">
-        <v>78</v>
+        <v>277</v>
       </c>
       <c r="AA31" t="s" s="2">
         <v>78</v>
@@ -5095,13 +5109,13 @@
         <v>78</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH31" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI31" t="s" s="2">
         <v>78</v>
@@ -5113,10 +5127,10 @@
         <v>78</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>78</v>
@@ -5127,10 +5141,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5141,7 +5155,7 @@
         <v>79</v>
       </c>
       <c r="G32" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H32" t="s" s="2">
         <v>78</v>
@@ -5153,16 +5167,20 @@
         <v>91</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>249</v>
+        <v>104</v>
       </c>
       <c r="L32" t="s" s="2">
+        <v>282</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>283</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>284</v>
+      </c>
+      <c r="O32" t="s" s="2">
         <v>285</v>
       </c>
-      <c r="M32" t="s" s="2">
-        <v>286</v>
-      </c>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
       <c r="P32" t="s" s="2">
         <v>78</v>
       </c>
@@ -5186,11 +5204,13 @@
         <v>78</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="Y32" s="2"/>
+        <v>78</v>
+      </c>
+      <c r="Y32" t="s" s="2">
+        <v>78</v>
+      </c>
       <c r="Z32" t="s" s="2">
-        <v>287</v>
+        <v>78</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>78</v>
@@ -5208,13 +5228,13 @@
         <v>78</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH32" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI32" t="s" s="2">
         <v>78</v>
@@ -5226,13 +5246,13 @@
         <v>78</v>
       </c>
       <c r="AL32" t="s" s="2">
+        <v>287</v>
+      </c>
+      <c r="AM32" t="s" s="2">
         <v>288</v>
       </c>
-      <c r="AM32" t="s" s="2">
-        <v>289</v>
-      </c>
       <c r="AN32" t="s" s="2">
-        <v>290</v>
+        <v>78</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>78</v>
@@ -5240,10 +5260,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5266,13 +5286,13 @@
         <v>91</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>292</v>
+        <v>255</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -5299,13 +5319,11 @@
         <v>78</v>
       </c>
       <c r="X33" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="Y33" t="s" s="2">
-        <v>78</v>
-      </c>
+        <v>276</v>
+      </c>
+      <c r="Y33" s="2"/>
       <c r="Z33" t="s" s="2">
-        <v>78</v>
+        <v>292</v>
       </c>
       <c r="AA33" t="s" s="2">
         <v>78</v>
@@ -5323,7 +5341,7 @@
         <v>78</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>79</v>
@@ -5341,24 +5359,24 @@
         <v>78</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>78</v>
+        <v>293</v>
       </c>
       <c r="AM33" t="s" s="2">
+        <v>294</v>
+      </c>
+      <c r="AN33" t="s" s="2">
         <v>295</v>
       </c>
-      <c r="AN33" t="s" s="2">
-        <v>296</v>
-      </c>
       <c r="AO33" t="s" s="2">
-        <v>297</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -5378,16 +5396,16 @@
         <v>78</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>297</v>
+      </c>
+      <c r="L34" t="s" s="2">
+        <v>298</v>
+      </c>
+      <c r="M34" t="s" s="2">
         <v>299</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>300</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>301</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -5438,7 +5456,7 @@
         <v>78</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>79</v>
@@ -5456,24 +5474,24 @@
         <v>78</v>
       </c>
       <c r="AL34" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AM34" t="s" s="2">
+        <v>300</v>
+      </c>
+      <c r="AN34" t="s" s="2">
+        <v>301</v>
+      </c>
+      <c r="AO34" t="s" s="2">
         <v>302</v>
-      </c>
-      <c r="AM34" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="AN34" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AO34" t="s" s="2">
-        <v>78</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -5496,18 +5514,16 @@
         <v>78</v>
       </c>
       <c r="K35" t="s" s="2">
+        <v>304</v>
+      </c>
+      <c r="L35" t="s" s="2">
         <v>305</v>
       </c>
-      <c r="L35" t="s" s="2">
+      <c r="M35" t="s" s="2">
         <v>306</v>
       </c>
-      <c r="M35" t="s" s="2">
-        <v>307</v>
-      </c>
       <c r="N35" s="2"/>
-      <c r="O35" t="s" s="2">
-        <v>308</v>
-      </c>
+      <c r="O35" s="2"/>
       <c r="P35" t="s" s="2">
         <v>78</v>
       </c>
@@ -5555,7 +5571,7 @@
         <v>78</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>79</v>
@@ -5564,22 +5580,22 @@
         <v>80</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>203</v>
+        <v>78</v>
       </c>
       <c r="AJ35" t="s" s="2">
-        <v>309</v>
+        <v>102</v>
       </c>
       <c r="AK35" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>312</v>
+        <v>78</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>78</v>
@@ -5587,10 +5603,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -5613,18 +5629,18 @@
         <v>78</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>316</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="O36" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="N36" s="2"/>
+      <c r="O36" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="P36" t="s" s="2">
         <v>78</v>
       </c>
@@ -5672,7 +5688,7 @@
         <v>78</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>79</v>
@@ -5681,22 +5697,22 @@
         <v>80</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>78</v>
+        <v>203</v>
       </c>
       <c r="AJ36" t="s" s="2">
-        <v>102</v>
+        <v>314</v>
       </c>
       <c r="AK36" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>78</v>
+        <v>315</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>78</v>
+        <v>317</v>
       </c>
       <c r="AO36" t="s" s="2">
         <v>78</v>
@@ -5704,10 +5720,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -5718,7 +5734,7 @@
         <v>79</v>
       </c>
       <c r="G37" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H37" t="s" s="2">
         <v>78</v>
@@ -5730,15 +5746,17 @@
         <v>78</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>104</v>
+        <v>319</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>105</v>
+        <v>320</v>
       </c>
       <c r="M37" t="s" s="2">
-        <v>106</v>
-      </c>
-      <c r="N37" s="2"/>
+        <v>321</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>322</v>
+      </c>
       <c r="O37" s="2"/>
       <c r="P37" t="s" s="2">
         <v>78</v>
@@ -5787,19 +5805,19 @@
         <v>78</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>107</v>
+        <v>318</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ37" t="s" s="2">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="AK37" t="s" s="2">
         <v>78</v>
@@ -5808,7 +5826,7 @@
         <v>78</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>108</v>
+        <v>323</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>78</v>
@@ -5819,21 +5837,21 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G38" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H38" t="s" s="2">
         <v>78</v>
@@ -5845,17 +5863,15 @@
         <v>78</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>114</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" t="s" s="2">
         <v>78</v>
@@ -5904,19 +5920,19 @@
         <v>78</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI38" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="AK38" t="s" s="2">
         <v>78</v>
@@ -5936,14 +5952,14 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
-        <v>322</v>
+        <v>110</v>
       </c>
       <c r="E39" s="2"/>
       <c r="F39" t="s" s="2">
@@ -5956,26 +5972,24 @@
         <v>78</v>
       </c>
       <c r="I39" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="K39" t="s" s="2">
         <v>111</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>323</v>
+        <v>112</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>324</v>
+        <v>113</v>
       </c>
       <c r="N39" t="s" s="2">
         <v>114</v>
       </c>
-      <c r="O39" t="s" s="2">
-        <v>207</v>
-      </c>
+      <c r="O39" s="2"/>
       <c r="P39" t="s" s="2">
         <v>78</v>
       </c>
@@ -6023,7 +6037,7 @@
         <v>78</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>325</v>
+        <v>118</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -6044,7 +6058,7 @@
         <v>78</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>78</v>
@@ -6062,7 +6076,7 @@
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
-        <v>78</v>
+        <v>327</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" t="s" s="2">
@@ -6075,22 +6089,26 @@
         <v>78</v>
       </c>
       <c r="I40" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>170</v>
+        <v>111</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>328</v>
-      </c>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
+        <v>329</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="O40" t="s" s="2">
+        <v>213</v>
+      </c>
       <c r="P40" t="s" s="2">
         <v>78</v>
       </c>
@@ -6114,31 +6132,31 @@
         <v>78</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>271</v>
+        <v>78</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>329</v>
+        <v>78</v>
       </c>
       <c r="Z40" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AF40" t="s" s="2">
         <v>330</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>326</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -6150,7 +6168,7 @@
         <v>78</v>
       </c>
       <c r="AJ40" t="s" s="2">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="AK40" t="s" s="2">
         <v>78</v>
@@ -6159,7 +6177,7 @@
         <v>78</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>318</v>
+        <v>193</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>78</v>
@@ -6184,7 +6202,7 @@
         <v>79</v>
       </c>
       <c r="G41" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H41" t="s" s="2">
         <v>78</v>
@@ -6196,7 +6214,7 @@
         <v>78</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>219</v>
+        <v>170</v>
       </c>
       <c r="L41" t="s" s="2">
         <v>332</v>
@@ -6229,13 +6247,13 @@
         <v>78</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>78</v>
+        <v>276</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>78</v>
+        <v>334</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>78</v>
+        <v>335</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>78</v>
@@ -6259,7 +6277,7 @@
         <v>79</v>
       </c>
       <c r="AH41" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI41" t="s" s="2">
         <v>78</v>
@@ -6274,7 +6292,7 @@
         <v>78</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>78</v>
@@ -6285,10 +6303,10 @@
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -6311,17 +6329,15 @@
         <v>78</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>335</v>
+        <v>225</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>337</v>
-      </c>
-      <c r="N42" t="s" s="2">
         <v>338</v>
       </c>
+      <c r="N42" s="2"/>
       <c r="O42" s="2"/>
       <c r="P42" t="s" s="2">
         <v>78</v>
@@ -6370,7 +6386,7 @@
         <v>78</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -6391,7 +6407,7 @@
         <v>78</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>78</v>
@@ -6428,16 +6444,16 @@
         <v>78</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>335</v>
+        <v>340</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>338</v>
+        <v>343</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -6508,7 +6524,7 @@
         <v>78</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>78</v>
@@ -6519,10 +6535,10 @@
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -6533,7 +6549,7 @@
         <v>79</v>
       </c>
       <c r="G44" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H44" t="s" s="2">
         <v>78</v>
@@ -6545,15 +6561,17 @@
         <v>78</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>314</v>
+        <v>340</v>
       </c>
       <c r="L44" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="N44" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="M44" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
         <v>78</v>
@@ -6602,13 +6620,13 @@
         <v>78</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH44" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI44" t="s" s="2">
         <v>78</v>
@@ -6623,7 +6641,7 @@
         <v>78</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>78</v>
@@ -6634,10 +6652,10 @@
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -6648,7 +6666,7 @@
         <v>79</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>78</v>
@@ -6660,13 +6678,13 @@
         <v>78</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>104</v>
+        <v>319</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>105</v>
+        <v>348</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>106</v>
+        <v>349</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -6717,19 +6735,19 @@
         <v>78</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>107</v>
+        <v>347</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH45" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI45" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ45" t="s" s="2">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="AK45" t="s" s="2">
         <v>78</v>
@@ -6738,7 +6756,7 @@
         <v>78</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>108</v>
+        <v>323</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>78</v>
@@ -6749,21 +6767,21 @@
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>110</v>
+        <v>78</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
         <v>79</v>
       </c>
       <c r="G46" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H46" t="s" s="2">
         <v>78</v>
@@ -6775,17 +6793,15 @@
         <v>78</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>113</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>114</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
         <v>78</v>
@@ -6834,19 +6850,19 @@
         <v>78</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH46" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI46" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ46" t="s" s="2">
-        <v>119</v>
+        <v>78</v>
       </c>
       <c r="AK46" t="s" s="2">
         <v>78</v>
@@ -6866,14 +6882,14 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
-        <v>322</v>
+        <v>110</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" t="s" s="2">
@@ -6886,26 +6902,24 @@
         <v>78</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="K47" t="s" s="2">
         <v>111</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>323</v>
+        <v>112</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>324</v>
+        <v>113</v>
       </c>
       <c r="N47" t="s" s="2">
         <v>114</v>
       </c>
-      <c r="O47" t="s" s="2">
-        <v>207</v>
-      </c>
+      <c r="O47" s="2"/>
       <c r="P47" t="s" s="2">
         <v>78</v>
       </c>
@@ -6953,7 +6967,7 @@
         <v>78</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>325</v>
+        <v>118</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -6974,7 +6988,7 @@
         <v>78</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>193</v>
+        <v>108</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>78</v>
@@ -6985,42 +6999,46 @@
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
-        <v>78</v>
+        <v>327</v>
       </c>
       <c r="E48" s="2"/>
       <c r="F48" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G48" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H48" t="s" s="2">
         <v>78</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>349</v>
+        <v>328</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
+        <v>329</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>114</v>
+      </c>
+      <c r="O48" t="s" s="2">
+        <v>213</v>
+      </c>
       <c r="P48" t="s" s="2">
         <v>78</v>
       </c>
@@ -7068,19 +7086,19 @@
         <v>78</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>348</v>
+        <v>330</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="AH48" t="s" s="2">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AI48" t="s" s="2">
         <v>78</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="AK48" t="s" s="2">
         <v>78</v>
@@ -7089,7 +7107,7 @@
         <v>78</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>108</v>
+        <v>193</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>78</v>
@@ -7100,10 +7118,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7111,7 +7129,7 @@
       </c>
       <c r="E49" s="2"/>
       <c r="F49" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>90</v>
@@ -7126,13 +7144,13 @@
         <v>78</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>229</v>
+        <v>104</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -7183,10 +7201,10 @@
         <v>78</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>90</v>
@@ -7204,7 +7222,7 @@
         <v>78</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>318</v>
+        <v>108</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>78</v>
@@ -7215,10 +7233,10 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7241,13 +7259,13 @@
         <v>78</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>104</v>
+        <v>235</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -7298,7 +7316,7 @@
         <v>78</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -7319,7 +7337,7 @@
         <v>78</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>78</v>
@@ -7330,10 +7348,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -7344,7 +7362,7 @@
         <v>79</v>
       </c>
       <c r="G51" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="H51" t="s" s="2">
         <v>78</v>
@@ -7356,18 +7374,16 @@
         <v>78</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>358</v>
+        <v>104</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="N51" s="2"/>
-      <c r="O51" t="s" s="2">
-        <v>361</v>
-      </c>
+      <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
         <v>78</v>
       </c>
@@ -7415,13 +7431,13 @@
         <v>78</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>79</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>78</v>
@@ -7436,12 +7452,129 @@
         <v>78</v>
       </c>
       <c r="AM51" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="AN51" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AO51" t="s" s="2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="B52" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="C52" s="2"/>
+      <c r="D52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="E52" s="2"/>
+      <c r="F52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>363</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>365</v>
+      </c>
+      <c r="N52" s="2"/>
+      <c r="O52" t="s" s="2">
+        <v>366</v>
+      </c>
+      <c r="P52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Q52" s="2"/>
+      <c r="R52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>362</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>79</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>102</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AM52" t="s" s="2">
         <v>108</v>
       </c>
-      <c r="AN51" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AO51" t="s" s="2">
+      <c r="AN52" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AO52" t="s" s="2">
         <v>78</v>
       </c>
     </row>

</xml_diff>